<commit_message>
Improve data transformation for UNFI West sales orders and store names
Adds item mapping and updates store name mapping in create_mappings.py, updates UNFIWestParser to extract item data, and adds get_item_mapping in mapping_utils.py.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a4c793ea-64cf-4601-8936-3568869ffe5a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/c5fd0f16-2d84-4af3-99b4-3191adee6a6a/a4c793ea-64cf-4601-8936-3568869ffe5a/Lu3JUaV
</commit_message>
<xml_diff>
--- a/mappings/unfi_west/store_mapping.xlsx
+++ b/mappings/unfi_west/store_mapping.xlsx
@@ -448,72 +448,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>UNFI WEST Distribution Center</t>
+          <t>KL - Richmond</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>UNFI West Distribution</t>
+          <t>KL - Richmond</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>UNFI West - Portland</t>
+          <t>UNFI WEST Distribution Center</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>UNFI West Portland</t>
+          <t>UNFI West Distribution</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>UNFI West - Seattle</t>
+          <t>UNFI West - Portland</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>UNFI West Seattle</t>
+          <t>UNFI West Portland</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>UNFI West Regional</t>
+          <t>UNFI West - Seattle</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>UNFI West Regional</t>
+          <t>UNFI West Seattle</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sample UNFI West Store</t>
+          <t>UNFI West Regional</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mapped UNFI West Store</t>
+          <t>UNFI West Regional</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Default Store Name</t>
+          <t>Sample UNFI West Store</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Default Mapped Store</t>
+          <t>Mapped UNFI West Store</t>
         </is>
       </c>
     </row>

</xml_diff>